<commit_message>
Lab is Working! (Figure out Beats and Tempo meaning)
</commit_message>
<xml_diff>
--- a/resources/LM4041 Voltage Reference Design.xlsx
+++ b/resources/LM4041 Voltage Reference Design.xlsx
@@ -1,17 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Keil_v5\ECE445L\Labs\lab-5-inside-the-oscilloscope\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B12315-5CF9-4553-9BEA-63BD2532355D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="24915" windowHeight="9015"/>
+    <workbookView minimized="1" xWindow="2148" yWindow="2928" windowWidth="21528" windowHeight="11388" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -111,7 +130,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -223,13 +242,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
+      <xdr:colOff>61594</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:rowOff>120014</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="110" name="Picture 109"/>
+        <xdr:cNvPr id="110" name="Picture 109">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -291,13 +316,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
+      <xdr:colOff>577215</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="111" name="Picture 110"/>
+        <xdr:cNvPr id="111" name="Picture 110">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -383,7 +414,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -416,9 +447,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -451,6 +499,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -626,30 +691,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.86328125" customWidth="1"/>
+    <col min="3" max="3" width="10.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -667,7 +732,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -681,7 +746,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -699,7 +764,7 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -711,7 +776,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -729,7 +794,7 @@
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -744,7 +809,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -758,7 +823,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -776,7 +841,7 @@
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -790,7 +855,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -805,7 +870,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -820,7 +885,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -835,7 +900,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -850,7 +915,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D16" s="6" t="s">
         <v>19</v>
       </c>
@@ -859,13 +924,13 @@
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
     </row>
-    <row r="17" spans="1:4" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:4" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:4" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -878,24 +943,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>